<commit_message>
update asset returns data
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM172"/>
+  <dimension ref="A1:ALM175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -15742,13 +15742,325 @@
         <v>-0.062821</v>
       </c>
     </row>
+    <row r="173" spans="1:34">
+      <c r="A173" s="3">
+        <v>44681</v>
+      </c>
+      <c r="B173" s="1">
+        <v>-0.1197008822896493</v>
+      </c>
+      <c r="C173" s="1">
+        <v>-0.09765014181108389</v>
+      </c>
+      <c r="D173" s="1">
+        <v>-0.09421284028863164</v>
+      </c>
+      <c r="E173" s="1">
+        <v>-0.0942131263232181</v>
+      </c>
+      <c r="F173" s="1">
+        <v>-0.0619020821609455</v>
+      </c>
+      <c r="G173" s="1">
+        <v>-0.08795671914903935</v>
+      </c>
+      <c r="H173" s="1">
+        <v>-0.08135645623700039</v>
+      </c>
+      <c r="I173" s="1">
+        <v>-0.08073192215432845</v>
+      </c>
+      <c r="J173" s="1">
+        <v>-0.09952152647786972</v>
+      </c>
+      <c r="K173" s="1">
+        <v>-0.09047183881294574</v>
+      </c>
+      <c r="L173" s="1">
+        <v>-0.06780709836223375</v>
+      </c>
+      <c r="M173" s="1">
+        <v>-0.05745364734320668</v>
+      </c>
+      <c r="N173" s="1">
+        <v>0.001714716129554983</v>
+      </c>
+      <c r="O173" s="1">
+        <v>-0.03637738552466607</v>
+      </c>
+      <c r="P173" s="1">
+        <v>0.01759276699943491</v>
+      </c>
+      <c r="Q173" s="1">
+        <v>0.01903609958843067</v>
+      </c>
+      <c r="R173" s="1">
+        <v>0.0277348443081904</v>
+      </c>
+      <c r="S173" s="1">
+        <v>0.07058499551981989</v>
+      </c>
+      <c r="T173" s="1">
+        <v>0.005875983963948173</v>
+      </c>
+      <c r="U173" s="1">
+        <v>-0.03852718341520267</v>
+      </c>
+      <c r="V173" s="1">
+        <v>-0.06533699999999999</v>
+      </c>
+      <c r="W173" s="1">
+        <v>-0.158923</v>
+      </c>
+      <c r="X173" s="1">
+        <v>0.03497</v>
+      </c>
+      <c r="Y173" s="1">
+        <v>-0.017101</v>
+      </c>
+      <c r="Z173" s="1">
+        <v>0.017311</v>
+      </c>
+      <c r="AA173" s="1">
+        <v>0.005639</v>
+      </c>
+      <c r="AB173" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC173" s="1">
+        <v>0.005196057706260364</v>
+      </c>
+      <c r="AD173" s="1">
+        <v>0.0008685919735187397</v>
+      </c>
+      <c r="AE173" s="1">
+        <v>0.5872791382517051</v>
+      </c>
+      <c r="AF173" s="1">
+        <v>0.4721365554995967</v>
+      </c>
+      <c r="AG173" s="1">
+        <v>-0.09371</v>
+      </c>
+      <c r="AH173" s="1">
+        <v>-0.120242</v>
+      </c>
+    </row>
+    <row r="174" spans="1:34">
+      <c r="A174" s="3">
+        <v>44712</v>
+      </c>
+      <c r="B174" s="1">
+        <v>-0.03471246104015158</v>
+      </c>
+      <c r="C174" s="1">
+        <v>0.01002700958481717</v>
+      </c>
+      <c r="D174" s="1">
+        <v>-0.02864143387839646</v>
+      </c>
+      <c r="E174" s="1">
+        <v>-0.02707440592130894</v>
+      </c>
+      <c r="F174" s="1">
+        <v>-0.001199760047990273</v>
+      </c>
+      <c r="G174" s="1">
+        <v>5.324388360872234E-05</v>
+      </c>
+      <c r="H174" s="1">
+        <v>-0.001315648568849692</v>
+      </c>
+      <c r="I174" s="1">
+        <v>-0.001880220323253301</v>
+      </c>
+      <c r="J174" s="1">
+        <v>-3.218706262486659E-05</v>
+      </c>
+      <c r="K174" s="1">
+        <v>-0.003054359324005329</v>
+      </c>
+      <c r="L174" s="1">
+        <v>0.002050449918866937</v>
+      </c>
+      <c r="M174" s="1">
+        <v>0.001375221847443209</v>
+      </c>
+      <c r="N174" s="1">
+        <v>-0.02510791749100161</v>
+      </c>
+      <c r="O174" s="1">
+        <v>0.00249881254775608</v>
+      </c>
+      <c r="P174" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q174" s="1">
+        <v>-0.009025587101296861</v>
+      </c>
+      <c r="R174" s="1">
+        <v>-0.001894176692981087</v>
+      </c>
+      <c r="S174" s="1">
+        <v>-0.002012097130104529</v>
+      </c>
+      <c r="T174" s="1">
+        <v>0</v>
+      </c>
+      <c r="U174" s="1">
+        <v>-0.04801593315004438</v>
+      </c>
+      <c r="V174" s="1">
+        <v>0.003061</v>
+      </c>
+      <c r="W174" s="1">
+        <v>-0.023615</v>
+      </c>
+      <c r="X174" s="1">
+        <v>-0.006725999999999999</v>
+      </c>
+      <c r="Y174" s="1">
+        <v>-0.000184</v>
+      </c>
+      <c r="Z174" s="1">
+        <v>0.001405</v>
+      </c>
+      <c r="AA174" s="1">
+        <v>0.023559</v>
+      </c>
+      <c r="AB174" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC174" s="1">
+        <v>-0.0095741829972988</v>
+      </c>
+      <c r="AD174" s="1">
+        <v>0.001295897660475998</v>
+      </c>
+      <c r="AE174" s="1">
+        <v>0.291178947625383</v>
+      </c>
+      <c r="AF174" s="1">
+        <v>0.2591606830265225</v>
+      </c>
+      <c r="AG174" s="1">
+        <v>0.010182</v>
+      </c>
+      <c r="AH174" s="1">
+        <v>-0.035145</v>
+      </c>
+    </row>
+    <row r="175" spans="1:34">
+      <c r="A175" s="3">
+        <v>44742</v>
+      </c>
+      <c r="B175" s="1">
+        <v>-0.01532130421019307</v>
+      </c>
+      <c r="C175" s="1">
+        <v>-0.04319098836865332</v>
+      </c>
+      <c r="D175" s="1">
+        <v>-0.009028777125059673</v>
+      </c>
+      <c r="E175" s="1">
+        <v>-0.01121121121121116</v>
+      </c>
+      <c r="F175" s="1">
+        <v>-0.004604604604604656</v>
+      </c>
+      <c r="G175" s="1">
+        <v>-0.08391999322386645</v>
+      </c>
+      <c r="H175" s="1">
+        <v>-0.08584427321885379</v>
+      </c>
+      <c r="I175" s="1">
+        <v>-0.08784248849818266</v>
+      </c>
+      <c r="J175" s="1">
+        <v>-0.08371748934976275</v>
+      </c>
+      <c r="K175" s="1">
+        <v>-0.0850205567826906</v>
+      </c>
+      <c r="L175" s="1">
+        <v>-0.0940148292089289</v>
+      </c>
+      <c r="M175" s="1">
+        <v>-0.07145044401347367</v>
+      </c>
+      <c r="N175" s="1">
+        <v>-0.02056951879490698</v>
+      </c>
+      <c r="O175" s="1">
+        <v>-0.06806196440342771</v>
+      </c>
+      <c r="P175" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q175" s="1">
+        <v>0.01373001390686412</v>
+      </c>
+      <c r="R175" s="1">
+        <v>-0.004234113832479403</v>
+      </c>
+      <c r="S175" s="1">
+        <v>0.02568247657480471</v>
+      </c>
+      <c r="T175" s="1">
+        <v>0</v>
+      </c>
+      <c r="U175" s="1">
+        <v>-0.07677089255258662</v>
+      </c>
+      <c r="V175" s="1">
+        <v>-0.07564799999999999</v>
+      </c>
+      <c r="W175" s="1">
+        <v>-0.034867</v>
+      </c>
+      <c r="X175" s="1">
+        <v>0.021364</v>
+      </c>
+      <c r="Y175" s="1">
+        <v>-0.037062</v>
+      </c>
+      <c r="Z175" s="1">
+        <v>0.026676</v>
+      </c>
+      <c r="AA175" s="1">
+        <v>-0.011929</v>
+      </c>
+      <c r="AB175" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC175" s="1">
+        <v>-0.002775486380016685</v>
+      </c>
+      <c r="AD175" s="1">
+        <v>0.000824210855066454</v>
+      </c>
+      <c r="AE175" s="1">
+        <v>0.5910289738620789</v>
+      </c>
+      <c r="AF175" s="1">
+        <v>0.5649993364820423</v>
+      </c>
+      <c r="AG175" s="1">
+        <v>-0.045019</v>
+      </c>
+      <c r="AH175" s="1">
+        <v>-0.014868</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A172">
+  <conditionalFormatting sqref="A1:A175">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH172">
+  <conditionalFormatting sqref="B2:AH175">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update LDI data 7/29/2022
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM175"/>
+  <dimension ref="A1:ALM176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16054,13 +16054,117 @@
         <v>-0.014868</v>
       </c>
     </row>
+    <row r="176" spans="1:34">
+      <c r="A176" s="3">
+        <v>44773</v>
+      </c>
+      <c r="B176" s="1">
+        <v>0.02436828907606237</v>
+      </c>
+      <c r="C176" s="1">
+        <v>0.04813090815554255</v>
+      </c>
+      <c r="D176" s="1">
+        <v>0.02571382144256562</v>
+      </c>
+      <c r="E176" s="1">
+        <v>0.02571370722818389</v>
+      </c>
+      <c r="F176" s="1">
+        <v>0.04055209171359619</v>
+      </c>
+      <c r="G176" s="1">
+        <v>0.09111634763220589</v>
+      </c>
+      <c r="H176" s="1">
+        <v>0.06861940110930509</v>
+      </c>
+      <c r="I176" s="1">
+        <v>0.07020923105436294</v>
+      </c>
+      <c r="J176" s="1">
+        <v>0.1037710993624084</v>
+      </c>
+      <c r="K176" s="1">
+        <v>0.09277966649736125</v>
+      </c>
+      <c r="L176" s="1">
+        <v>0.04927746603982053</v>
+      </c>
+      <c r="M176" s="1">
+        <v>-0.006885386790850156</v>
+      </c>
+      <c r="N176" s="1">
+        <v>0.01866284928785999</v>
+      </c>
+      <c r="O176" s="1">
+        <v>0.06022693781314481</v>
+      </c>
+      <c r="P176" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q176" s="1">
+        <v>-0.01484453678225639</v>
+      </c>
+      <c r="R176" s="1">
+        <v>-0.004227422915525914</v>
+      </c>
+      <c r="S176" s="1">
+        <v>-0.0440746449675008</v>
+      </c>
+      <c r="T176" s="1">
+        <v>0</v>
+      </c>
+      <c r="U176" s="1">
+        <v>0.08396758540850757</v>
+      </c>
+      <c r="V176" s="1">
+        <v>0.059062</v>
+      </c>
+      <c r="W176" s="1">
+        <v>0.07610599999999999</v>
+      </c>
+      <c r="X176" s="1">
+        <v>-0.033578</v>
+      </c>
+      <c r="Y176" s="1">
+        <v>0.032877</v>
+      </c>
+      <c r="Z176" s="1">
+        <v>-0.001731</v>
+      </c>
+      <c r="AA176" s="1">
+        <v>0.019184</v>
+      </c>
+      <c r="AB176" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC176" s="1">
+        <v>-0.007313718654653281</v>
+      </c>
+      <c r="AD176" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE176" s="1">
+        <v>0.4000249543988068</v>
+      </c>
+      <c r="AF176" s="1">
+        <v>0.4428207655525018</v>
+      </c>
+      <c r="AG176" s="1">
+        <v>0.051304</v>
+      </c>
+      <c r="AH176" s="1">
+        <v>0.053141</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A175">
+  <conditionalFormatting sqref="A1:A176">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH175">
+  <conditionalFormatting sqref="B2:AH176">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update LDI data 8/31/2022
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM176"/>
+  <dimension ref="A1:ALM177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16158,13 +16158,117 @@
         <v>0.053141</v>
       </c>
     </row>
+    <row r="177" spans="1:34">
+      <c r="A177" s="3">
+        <v>44804</v>
+      </c>
+      <c r="B177" s="1">
+        <v>-0.0492719055987948</v>
+      </c>
+      <c r="C177" s="1">
+        <v>-0.04501219989900274</v>
+      </c>
+      <c r="D177" s="1">
+        <v>-0.05448194922591543</v>
+      </c>
+      <c r="E177" s="1">
+        <v>-0.05448085274378212</v>
+      </c>
+      <c r="F177" s="1">
+        <v>-0.05068979680591457</v>
+      </c>
+      <c r="G177" s="1">
+        <v>-0.04244011921681046</v>
+      </c>
+      <c r="H177" s="1">
+        <v>-0.03859060402684567</v>
+      </c>
+      <c r="I177" s="1">
+        <v>-0.03723930630118</v>
+      </c>
+      <c r="J177" s="1">
+        <v>-0.02180901004121516</v>
+      </c>
+      <c r="K177" s="1">
+        <v>-0.03889256075731495</v>
+      </c>
+      <c r="L177" s="1">
+        <v>-0.04994683212372109</v>
+      </c>
+      <c r="M177" s="1">
+        <v>0.0003320654470808648</v>
+      </c>
+      <c r="N177" s="1">
+        <v>0.01534197588255681</v>
+      </c>
+      <c r="O177" s="1">
+        <v>-0.02394818407994781</v>
+      </c>
+      <c r="P177" s="1">
+        <v>0.00529394343254852</v>
+      </c>
+      <c r="Q177" s="1">
+        <v>0.0124522075099609</v>
+      </c>
+      <c r="R177" s="1">
+        <v>-0.008030591048697189</v>
+      </c>
+      <c r="S177" s="1">
+        <v>0.03991546346575769</v>
+      </c>
+      <c r="T177" s="1">
+        <v>0</v>
+      </c>
+      <c r="U177" s="1">
+        <v>-0.05985275404471913</v>
+      </c>
+      <c r="V177" s="1">
+        <v>-0.03325</v>
+      </c>
+      <c r="W177" s="1">
+        <v>-0.08456200000000001</v>
+      </c>
+      <c r="X177" s="1">
+        <v>0.014346</v>
+      </c>
+      <c r="Y177" s="1">
+        <v>-0.011882</v>
+      </c>
+      <c r="Z177" s="1">
+        <v>-0.002761</v>
+      </c>
+      <c r="AA177" s="1">
+        <v>0.005754</v>
+      </c>
+      <c r="AB177" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC177" s="1">
+        <v>0.002715131471644762</v>
+      </c>
+      <c r="AD177" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE177" s="1">
+        <v>0.1750044560632167</v>
+      </c>
+      <c r="AF177" s="1">
+        <v>0.1439047713525086</v>
+      </c>
+      <c r="AG177" s="1">
+        <v>-0.045252</v>
+      </c>
+      <c r="AH177" s="1">
+        <v>-0.048169</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A176">
+  <conditionalFormatting sqref="A1:A177">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH176">
+  <conditionalFormatting sqref="B2:AH177">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update data for quarterly review using GT Total consolidation
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM177"/>
+  <dimension ref="A1:ALM178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16262,13 +16262,117 @@
         <v>-0.048169</v>
       </c>
     </row>
+    <row r="178" spans="1:34">
+      <c r="A178" s="3">
+        <v>44834</v>
+      </c>
+      <c r="B178" s="1">
+        <v>-0.1033207895952994</v>
+      </c>
+      <c r="C178" s="1">
+        <v>-0.08738840471560338</v>
+      </c>
+      <c r="D178" s="1">
+        <v>-0.08361218554563754</v>
+      </c>
+      <c r="E178" s="1">
+        <v>-0.0847599164926931</v>
+      </c>
+      <c r="F178" s="1">
+        <v>-0.06706370415616814</v>
+      </c>
+      <c r="G178" s="1">
+        <v>-0.09339570164348932</v>
+      </c>
+      <c r="H178" s="1">
+        <v>-0.09743765392833259</v>
+      </c>
+      <c r="I178" s="1">
+        <v>-0.09825713239498146</v>
+      </c>
+      <c r="J178" s="1">
+        <v>-0.09728189402504728</v>
+      </c>
+      <c r="K178" s="1">
+        <v>-0.09401707910872559</v>
+      </c>
+      <c r="L178" s="1">
+        <v>-0.09726704699809829</v>
+      </c>
+      <c r="M178" s="1">
+        <v>-0.1190210338896098</v>
+      </c>
+      <c r="N178" s="1">
+        <v>-0.02165833550055563</v>
+      </c>
+      <c r="O178" s="1">
+        <v>-0.04021417179311915</v>
+      </c>
+      <c r="P178" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q178" s="1">
+        <v>0.02985323814218255</v>
+      </c>
+      <c r="R178" s="1">
+        <v>0.03031856333458149</v>
+      </c>
+      <c r="S178" s="1">
+        <v>0.0575868652098519</v>
+      </c>
+      <c r="T178" s="1">
+        <v>0</v>
+      </c>
+      <c r="U178" s="1">
+        <v>-0.1324261613573743</v>
+      </c>
+      <c r="V178" s="1">
+        <v>-0.08886200000000001</v>
+      </c>
+      <c r="W178" s="1">
+        <v>-0.147842</v>
+      </c>
+      <c r="X178" s="1">
+        <v>0.040747</v>
+      </c>
+      <c r="Y178" s="1">
+        <v>-0.013409</v>
+      </c>
+      <c r="Z178" s="1">
+        <v>0.004026</v>
+      </c>
+      <c r="AA178" s="1">
+        <v>-0.009649999999999999</v>
+      </c>
+      <c r="AB178" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC178" s="1">
+        <v>0.009664615045574792</v>
+      </c>
+      <c r="AD178" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE178" s="1">
+        <v>0.1555200797483305</v>
+      </c>
+      <c r="AF178" s="1">
+        <v>0.1365453266851242</v>
+      </c>
+      <c r="AG178" s="1">
+        <v>-0.085727</v>
+      </c>
+      <c r="AH178" s="1">
+        <v>-0.100014</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A177">
+  <conditionalFormatting sqref="A1:A178">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH177">
+  <conditionalFormatting sqref="B2:AH178">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update LDI Data 10/31/2022
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM178"/>
+  <dimension ref="A1:ALM179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16366,13 +16366,117 @@
         <v>-0.100014</v>
       </c>
     </row>
+    <row r="179" spans="1:34">
+      <c r="A179" s="3">
+        <v>44865</v>
+      </c>
+      <c r="B179" s="1">
+        <v>-0.08518627595346773</v>
+      </c>
+      <c r="C179" s="1">
+        <v>-0.02247835963750866</v>
+      </c>
+      <c r="D179" s="1">
+        <v>-0.06820238475460449</v>
+      </c>
+      <c r="E179" s="1">
+        <v>-0.06820255474452552</v>
+      </c>
+      <c r="F179" s="1">
+        <v>-0.04373090353557407</v>
+      </c>
+      <c r="G179" s="1">
+        <v>0.07986345457689326</v>
+      </c>
+      <c r="H179" s="1">
+        <v>0.05963460252633856</v>
+      </c>
+      <c r="I179" s="1">
+        <v>0.0608187051179756</v>
+      </c>
+      <c r="J179" s="1">
+        <v>0.1094162607916307</v>
+      </c>
+      <c r="K179" s="1">
+        <v>0.0809579276187542</v>
+      </c>
+      <c r="L179" s="1">
+        <v>0.05327780051520326</v>
+      </c>
+      <c r="M179" s="1">
+        <v>-0.03154865892508474</v>
+      </c>
+      <c r="N179" s="1">
+        <v>0.008497065187643704</v>
+      </c>
+      <c r="O179" s="1">
+        <v>0.02846439169139448</v>
+      </c>
+      <c r="P179" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q179" s="1">
+        <v>0.00146676239221244</v>
+      </c>
+      <c r="R179" s="1">
+        <v>0.005376809760581303</v>
+      </c>
+      <c r="S179" s="1">
+        <v>0.001892027978815491</v>
+      </c>
+      <c r="T179" s="1">
+        <v>0</v>
+      </c>
+      <c r="U179" s="1">
+        <v>0.03284580025073125</v>
+      </c>
+      <c r="V179" s="1">
+        <v>0.059597</v>
+      </c>
+      <c r="W179" s="1">
+        <v>-0.07781399999999999</v>
+      </c>
+      <c r="X179" s="1">
+        <v>-0.017756</v>
+      </c>
+      <c r="Y179" s="1">
+        <v>0.019767</v>
+      </c>
+      <c r="Z179" s="1">
+        <v>0.018137</v>
+      </c>
+      <c r="AA179" s="1">
+        <v>-6.600000000000001E-05</v>
+      </c>
+      <c r="AB179" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC179" s="1">
+        <v>-0.008332736387956374</v>
+      </c>
+      <c r="AD179" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE179" s="1">
+        <v>0.2392742162348014</v>
+      </c>
+      <c r="AF179" s="1">
+        <v>0.2471914361383127</v>
+      </c>
+      <c r="AG179" s="1">
+        <v>-0.020832</v>
+      </c>
+      <c r="AH179" s="1">
+        <v>-0.08355499999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A178">
+  <conditionalFormatting sqref="A1:A179">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH178">
+  <conditionalFormatting sqref="B2:AH179">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update asset return data 11/30
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM179"/>
+  <dimension ref="A1:ALM180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16470,13 +16470,117 @@
         <v>-0.08355499999999999</v>
       </c>
     </row>
+    <row r="180" spans="1:34">
+      <c r="A180" s="3">
+        <v>44895</v>
+      </c>
+      <c r="B180" s="1">
+        <v>0.0971428571428572</v>
+      </c>
+      <c r="C180" s="1">
+        <v>0.09077890818239998</v>
+      </c>
+      <c r="D180" s="1">
+        <v>0.06320955119635219</v>
+      </c>
+      <c r="E180" s="1">
+        <v>0.06438188494492048</v>
+      </c>
+      <c r="F180" s="1">
+        <v>0.05862550994208782</v>
+      </c>
+      <c r="G180" s="1">
+        <v>0.05375286029369986</v>
+      </c>
+      <c r="H180" s="1">
+        <v>0.07597591964118222</v>
+      </c>
+      <c r="I180" s="1">
+        <v>0.07455088815016286</v>
+      </c>
+      <c r="J180" s="1">
+        <v>0.02150348997191442</v>
+      </c>
+      <c r="K180" s="1">
+        <v>0.05015475492350419</v>
+      </c>
+      <c r="L180" s="1">
+        <v>0.1108742857142857</v>
+      </c>
+      <c r="M180" s="1">
+        <v>0.1463521033767214</v>
+      </c>
+      <c r="N180" s="1">
+        <v>0.01109882463139722</v>
+      </c>
+      <c r="O180" s="1">
+        <v>0.01871794686844064</v>
+      </c>
+      <c r="P180" s="1">
+        <v>0.01820209087747293</v>
+      </c>
+      <c r="Q180" s="1">
+        <v>-0.02390404464760609</v>
+      </c>
+      <c r="R180" s="1">
+        <v>-0.0201499607198482</v>
+      </c>
+      <c r="S180" s="1">
+        <v>-0.06032641182414533</v>
+      </c>
+      <c r="T180" s="1">
+        <v>0</v>
+      </c>
+      <c r="U180" s="1">
+        <v>0.0582618546690401</v>
+      </c>
+      <c r="V180" s="1">
+        <v>0.07105800000000001</v>
+      </c>
+      <c r="W180" s="1">
+        <v>0.121817</v>
+      </c>
+      <c r="X180" s="1">
+        <v>-0.046014</v>
+      </c>
+      <c r="Y180" s="1">
+        <v>0.021424</v>
+      </c>
+      <c r="Z180" s="1">
+        <v>-0.002828</v>
+      </c>
+      <c r="AA180" s="1">
+        <v>0.010457</v>
+      </c>
+      <c r="AB180" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC180" s="1">
+        <v>-0.003035182531829058</v>
+      </c>
+      <c r="AD180" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE180" s="1">
+        <v>0.04375997841006241</v>
+      </c>
+      <c r="AF180" s="1">
+        <v>0.05340392030250962</v>
+      </c>
+      <c r="AG180" s="1">
+        <v>0.08726800000000001</v>
+      </c>
+      <c r="AH180" s="1">
+        <v>0.09778100000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A179">
+  <conditionalFormatting sqref="A1:A180">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH179">
+  <conditionalFormatting sqref="B2:AH180">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update asset return to be consistent with index returns
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -61,13 +61,13 @@
     <t>CDLI</t>
   </si>
   <si>
-    <t>HF MACRO</t>
+    <t>HFRX MACRO/CTA</t>
   </si>
   <si>
     <t>HFRI MACRO</t>
   </si>
   <si>
-    <t>TREND</t>
+    <t>SG TREND</t>
   </si>
   <si>
     <t>ALT RISK</t>

</xml_diff>

<commit_message>
Update LDI data 12/31/2022
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM180"/>
+  <dimension ref="A1:ALM181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16574,13 +16574,117 @@
         <v>0.09778100000000001</v>
       </c>
     </row>
+    <row r="181" spans="1:34">
+      <c r="A181" s="3">
+        <v>44926</v>
+      </c>
+      <c r="B181" s="1">
+        <v>-0.02259389671361489</v>
+      </c>
+      <c r="C181" s="1">
+        <v>-0.01146252586940244</v>
+      </c>
+      <c r="D181" s="1">
+        <v>-0.01444605637553786</v>
+      </c>
+      <c r="E181" s="1">
+        <v>-0.01149954001839926</v>
+      </c>
+      <c r="F181" s="1">
+        <v>-0.00948582515899532</v>
+      </c>
+      <c r="G181" s="1">
+        <v>-0.05897144929916109</v>
+      </c>
+      <c r="H181" s="1">
+        <v>-0.04048056805934186</v>
+      </c>
+      <c r="I181" s="1">
+        <v>-0.03957976575878397</v>
+      </c>
+      <c r="J181" s="1">
+        <v>-0.06643301598609541</v>
+      </c>
+      <c r="K181" s="1">
+        <v>-0.05991315471579395</v>
+      </c>
+      <c r="L181" s="1">
+        <v>-5.14395353981012E-05</v>
+      </c>
+      <c r="M181" s="1">
+        <v>-0.01636343066369084</v>
+      </c>
+      <c r="N181" s="1">
+        <v>0.003564127227706271</v>
+      </c>
+      <c r="O181" s="1">
+        <v>-0.007533703409991932</v>
+      </c>
+      <c r="P181" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q181" s="1">
+        <v>0.0004975281537757947</v>
+      </c>
+      <c r="R181" s="1">
+        <v>0.0004682066729762013</v>
+      </c>
+      <c r="S181" s="1">
+        <v>-0.002330336020999524</v>
+      </c>
+      <c r="T181" s="1">
+        <v>0</v>
+      </c>
+      <c r="U181" s="1">
+        <v>-0.05625223020849257</v>
+      </c>
+      <c r="V181" s="1">
+        <v>-0.029681</v>
+      </c>
+      <c r="W181" s="1">
+        <v>-0.031054</v>
+      </c>
+      <c r="X181" s="1">
+        <v>-0.001305</v>
+      </c>
+      <c r="Y181" s="1">
+        <v>0.00685</v>
+      </c>
+      <c r="Z181" s="1">
+        <v>0.014334</v>
+      </c>
+      <c r="AA181" s="1">
+        <v>-0.006806</v>
+      </c>
+      <c r="AB181" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC181" s="1">
+        <v>-0.02294225919023719</v>
+      </c>
+      <c r="AD181" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE181" s="1">
+        <v>0.04082101147569905</v>
+      </c>
+      <c r="AF181" s="1">
+        <v>0.01533792375253373</v>
+      </c>
+      <c r="AG181" s="1">
+        <v>-0.01146</v>
+      </c>
+      <c r="AH181" s="1">
+        <v>-0.022407</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A180">
+  <conditionalFormatting sqref="A1:A181">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH180">
+  <conditionalFormatting sqref="B2:AH181">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update asset data 3/31/23
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM183"/>
+  <dimension ref="A1:ALM184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16886,13 +16886,117 @@
         <v>-0.062184</v>
       </c>
     </row>
+    <row r="184" spans="1:34">
+      <c r="A184" s="3">
+        <v>45016</v>
+      </c>
+      <c r="B184" s="1">
+        <v>0.05492813141683772</v>
+      </c>
+      <c r="C184" s="1">
+        <v>0.04319771889207691</v>
+      </c>
+      <c r="D184" s="1">
+        <v>0.04488695689232669</v>
+      </c>
+      <c r="E184" s="1">
+        <v>0.04876915931258718</v>
+      </c>
+      <c r="F184" s="1">
+        <v>0.05172696022262224</v>
+      </c>
+      <c r="G184" s="1">
+        <v>0.03505157235872702</v>
+      </c>
+      <c r="H184" s="1">
+        <v>0.02820260087119641</v>
+      </c>
+      <c r="I184" s="1">
+        <v>0.02196491359551334</v>
+      </c>
+      <c r="J184" s="1">
+        <v>-0.04981942455182975</v>
+      </c>
+      <c r="K184" s="1">
+        <v>0.02507108832280069</v>
+      </c>
+      <c r="L184" s="1">
+        <v>0.01894638431311435</v>
+      </c>
+      <c r="M184" s="1">
+        <v>0.02725075466022142</v>
+      </c>
+      <c r="N184" s="1">
+        <v>-0.0009748276829143476</v>
+      </c>
+      <c r="O184" s="1">
+        <v>0.01125455607801662</v>
+      </c>
+      <c r="P184" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q184" s="1">
+        <v>-0.03015170074437001</v>
+      </c>
+      <c r="R184" s="1">
+        <v>0</v>
+      </c>
+      <c r="S184" s="1">
+        <v>-0.07688647825673234</v>
+      </c>
+      <c r="T184" s="1">
+        <v>0</v>
+      </c>
+      <c r="U184" s="1">
+        <v>-0.02433796042140468</v>
+      </c>
+      <c r="V184" s="1">
+        <v>0.01457</v>
+      </c>
+      <c r="W184" s="1">
+        <v>0.076304</v>
+      </c>
+      <c r="X184" s="1">
+        <v>-0.027278</v>
+      </c>
+      <c r="Y184" s="1">
+        <v>0.004489</v>
+      </c>
+      <c r="Z184" s="1">
+        <v>0.005325</v>
+      </c>
+      <c r="AA184" s="1">
+        <v>-0.003178</v>
+      </c>
+      <c r="AB184" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC184" s="1">
+        <v>-0.009837630804631214</v>
+      </c>
+      <c r="AD184" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE184" s="1">
+        <v>-0.006826858874488528</v>
+      </c>
+      <c r="AF184" s="1">
+        <v>-0.01597829501976</v>
+      </c>
+      <c r="AG184" s="1">
+        <v>0.042123</v>
+      </c>
+      <c r="AH184" s="1">
+        <v>0.053061</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A183">
+  <conditionalFormatting sqref="A1:A184">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH183">
+  <conditionalFormatting sqref="B2:AH184">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update LDI Date 4/28/2023
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM184"/>
+  <dimension ref="A1:ALM185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16990,13 +16990,117 @@
         <v>0.053061</v>
       </c>
     </row>
+    <row r="185" spans="1:34">
+      <c r="A185" s="3">
+        <v>45046</v>
+      </c>
+      <c r="B185" s="1">
+        <v>0.002711157455683066</v>
+      </c>
+      <c r="C185" s="1">
+        <v>0.007512953998991545</v>
+      </c>
+      <c r="D185" s="1">
+        <v>0.001992887239290253</v>
+      </c>
+      <c r="E185" s="1">
+        <v>0.001992914083259523</v>
+      </c>
+      <c r="F185" s="1">
+        <v>0.007704280155642174</v>
+      </c>
+      <c r="G185" s="1">
+        <v>0.01464236088297044</v>
+      </c>
+      <c r="H185" s="1">
+        <v>0.01274042921640173</v>
+      </c>
+      <c r="I185" s="1">
+        <v>0.01108558019017836</v>
+      </c>
+      <c r="J185" s="1">
+        <v>-0.01858379880209748</v>
+      </c>
+      <c r="K185" s="1">
+        <v>0.009734307581129809</v>
+      </c>
+      <c r="L185" s="1">
+        <v>0.02449106374844701</v>
+      </c>
+      <c r="M185" s="1">
+        <v>-0.01335985781799087</v>
+      </c>
+      <c r="N185" s="1">
+        <v>0.009474909102306972</v>
+      </c>
+      <c r="O185" s="1">
+        <v>0.009650438156030283</v>
+      </c>
+      <c r="P185" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q185" s="1">
+        <v>0.01364195731727058</v>
+      </c>
+      <c r="R185" s="1">
+        <v>-0.0203482412164997</v>
+      </c>
+      <c r="S185" s="1">
+        <v>0.02834452842699409</v>
+      </c>
+      <c r="T185" s="1">
+        <v>0</v>
+      </c>
+      <c r="U185" s="1">
+        <v>0.001178929317828592</v>
+      </c>
+      <c r="V185" s="1">
+        <v>0.017551</v>
+      </c>
+      <c r="W185" s="1">
+        <v>0.00729</v>
+      </c>
+      <c r="X185" s="1">
+        <v>0.011509</v>
+      </c>
+      <c r="Y185" s="1">
+        <v>0.009399999999999999</v>
+      </c>
+      <c r="Z185" s="1">
+        <v>0.022814</v>
+      </c>
+      <c r="AA185" s="1">
+        <v>-0.005809999999999999</v>
+      </c>
+      <c r="AB185" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC185" s="1">
+        <v>0.001679542418934051</v>
+      </c>
+      <c r="AD185" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE185" s="1">
+        <v>0.06681577824608587</v>
+      </c>
+      <c r="AF185" s="1">
+        <v>0.08450438616268041</v>
+      </c>
+      <c r="AG185" s="1">
+        <v>0.007114000000000001</v>
+      </c>
+      <c r="AH185" s="1">
+        <v>0.003357</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A184">
+  <conditionalFormatting sqref="A1:A185">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH184">
+  <conditionalFormatting sqref="B2:AH185">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated June LDI Data
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -500,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ALM186"/>
+  <dimension ref="A1:ALM187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17198,13 +17198,117 @@
         <v>-0.037948</v>
       </c>
     </row>
+    <row r="187" spans="1:34">
+      <c r="A187" s="3">
+        <v>45107</v>
+      </c>
+      <c r="B187" s="1">
+        <v>0.007789397764154327</v>
+      </c>
+      <c r="C187" s="1">
+        <v>0.01538966594377356</v>
+      </c>
+      <c r="D187" s="1">
+        <v>-0.004794405705917382</v>
+      </c>
+      <c r="E187" s="1">
+        <v>-0.001145737855178686</v>
+      </c>
+      <c r="F187" s="1">
+        <v>-0.006876564352522707</v>
+      </c>
+      <c r="G187" s="1">
+        <v>0.0647275128414313</v>
+      </c>
+      <c r="H187" s="1">
+        <v>0.05642279189937649</v>
+      </c>
+      <c r="I187" s="1">
+        <v>0.05664485345076065</v>
+      </c>
+      <c r="J187" s="1">
+        <v>0.07949246992255588</v>
+      </c>
+      <c r="K187" s="1">
+        <v>0.06690879839484687</v>
+      </c>
+      <c r="L187" s="1">
+        <v>0.04403445962161023</v>
+      </c>
+      <c r="M187" s="1">
+        <v>0.0322890259042492</v>
+      </c>
+      <c r="N187" s="1">
+        <v>0.02237769898193842</v>
+      </c>
+      <c r="O187" s="1">
+        <v>0.01628023742872653</v>
+      </c>
+      <c r="P187" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q187" s="1">
+        <v>0.00548615399230501</v>
+      </c>
+      <c r="R187" s="1">
+        <v>0.01345777622507449</v>
+      </c>
+      <c r="S187" s="1">
+        <v>0.01947923505546867</v>
+      </c>
+      <c r="T187" s="1">
+        <v>0</v>
+      </c>
+      <c r="U187" s="1">
+        <v>0.04513403100341362</v>
+      </c>
+      <c r="V187" s="1">
+        <v>0.049303</v>
+      </c>
+      <c r="W187" s="1">
+        <v>-0.004797</v>
+      </c>
+      <c r="X187" s="1">
+        <v>0.010189</v>
+      </c>
+      <c r="Y187" s="1">
+        <v>0.013751</v>
+      </c>
+      <c r="Z187" s="1">
+        <v>0.004007</v>
+      </c>
+      <c r="AA187" s="1">
+        <v>-0.007897999999999999</v>
+      </c>
+      <c r="AB187" s="1">
+        <v>0.001666666666666667</v>
+      </c>
+      <c r="AC187" s="1">
+        <v>-0.002682680850675857</v>
+      </c>
+      <c r="AD187" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE187" s="1">
+        <v>0.0120712203943667</v>
+      </c>
+      <c r="AF187" s="1">
+        <v>-0.02294190830964304</v>
+      </c>
+      <c r="AG187" s="1">
+        <v>0.014455</v>
+      </c>
+      <c r="AH187" s="1">
+        <v>0.007095000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A186">
+  <conditionalFormatting sqref="A1:A187">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AH186">
+  <conditionalFormatting sqref="B2:AH187">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update ldi data 12/30/2023 and new PBO Cashflows
</commit_message>
<xml_diff>
--- a/data/time_series/asset_return_data.xlsx
+++ b/data/time_series/asset_return_data.xlsx
@@ -17783,22 +17783,22 @@
         <v>0</v>
       </c>
       <c r="V192" s="1">
-        <v>0.08839999999999999</v>
+        <v>0.088147</v>
       </c>
       <c r="W192" s="1">
-        <v>0.164367</v>
+        <v>0.163541</v>
       </c>
       <c r="X192" s="1">
-        <v>-0.017576</v>
+        <v>-0.034378</v>
       </c>
       <c r="Y192" s="1">
-        <v>0.027594</v>
+        <v>0.028122</v>
       </c>
       <c r="Z192" s="1">
         <v>-0.001465</v>
       </c>
       <c r="AA192" s="1">
-        <v>0.005121</v>
+        <v>0.003736</v>
       </c>
       <c r="AB192" s="1">
         <v>0.001666666666666667</v>
@@ -17816,10 +17816,10 @@
         <v>-0.008565018648328038</v>
       </c>
       <c r="AG192" s="1">
-        <v>0.106704</v>
+        <v>0.1066</v>
       </c>
       <c r="AH192" s="1">
-        <v>0.145011</v>
+        <v>0.142069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>